<commit_message>
Add director data hook and update PDF documents
Introduces useReadDataDirectorMain hook to fetch principal director data. Updates AcademicTranscriptDocument and FinalRecordDocument to display director's degree and name dynamically in signatures. Also updates index.js exports and modifies the Excel template.
</commit_message>
<xml_diff>
--- a/public/templates/Carga-de-Horarios.xlsx
+++ b/public/templates/Carga-de-Horarios.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UNET\Documents\GitHub\SGAuni-Frontend\public\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4E4375-6DCC-4FF3-AB6B-4CEDDD2CF8DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="W/VtXsGZO7mGxjItgSRku3W/7b8sCAIwQLfwOJnvPsY="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Código Curso</t>
   </si>
@@ -71,30 +80,37 @@
   <si>
     <t>german@uni.edu</t>
   </si>
+  <si>
+    <t>Código Grupo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,48 +118,57 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -333,55 +358,64 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="12.63"/>
-    <col customWidth="1" min="7" max="7" width="17.0"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="6" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -396,39 +430,39 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2">
-        <v>1.0</v>
+      <c r="D2" s="2">
+        <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>4.0</v>
+      <c r="E2" s="2">
+        <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2">
-        <v>40.0</v>
+      <c r="G2" s="2">
+        <v>40</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0.3333333333333333</v>
+      <c r="I2" s="2">
+        <v>1</v>
       </c>
       <c r="J2" s="4">
-        <v>0.4166666666666667</v>
+        <v>0.33333333333333331</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="4">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -443,39 +477,39 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
+      <c r="D3" s="2">
+        <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <v>4.0</v>
+      <c r="E3" s="2">
+        <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2">
-        <v>40.0</v>
+      <c r="G3" s="2">
+        <v>40</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.3333333333333333</v>
+      <c r="I3" s="2">
+        <v>3</v>
       </c>
       <c r="J3" s="4">
-        <v>0.4166666666666667</v>
+        <v>0.33333333333333331</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="4">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -490,39 +524,39 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2">
-        <v>2.0</v>
+      <c r="D4" s="2">
+        <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <v>3.0</v>
+      <c r="E4" s="2">
+        <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2">
-        <v>35.0</v>
+      <c r="G4" s="2">
+        <v>35</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2">
-        <v>2.0</v>
+      <c r="I4" s="2">
+        <v>2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>0.375</v>
       </c>
-      <c r="J4" s="4">
-        <v>0.4583333333333333</v>
+      <c r="K4" s="4">
+        <v>0.45833333333333331</v>
       </c>
-      <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -537,9 +571,9 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2"/>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -564,16 +598,16 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -591,9 +625,9 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="2"/>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -618,9 +652,9 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2"/>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -645,9 +679,9 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2"/>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -672,9 +706,9 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="2"/>
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -699,9 +733,9 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2"/>
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -726,9 +760,9 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="2"/>
+      <c r="Z11" s="2"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -753,9 +787,9 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="2"/>
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -780,9 +814,9 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="2"/>
+      <c r="Z13" s="2"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -807,9 +841,9 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2"/>
+      <c r="Z14" s="2"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -834,9 +868,9 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="2"/>
+      <c r="Z15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -861,9 +895,9 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2"/>
+      <c r="Z16" s="2"/>
+    </row>
+    <row r="17" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -888,9 +922,9 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2"/>
+      <c r="Z17" s="2"/>
+    </row>
+    <row r="18" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -915,9 +949,9 @@
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2"/>
+      <c r="Z18" s="2"/>
+    </row>
+    <row r="19" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -942,9 +976,9 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2"/>
+      <c r="Z19" s="2"/>
+    </row>
+    <row r="20" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -969,9 +1003,9 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2"/>
+      <c r="Z20" s="2"/>
+    </row>
+    <row r="21" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -996,9 +1030,9 @@
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2"/>
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1023,9 +1057,9 @@
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2"/>
+      <c r="Z22" s="2"/>
+    </row>
+    <row r="23" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1050,9 +1084,9 @@
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2"/>
+      <c r="Z23" s="2"/>
+    </row>
+    <row r="24" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1077,9 +1111,9 @@
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2"/>
+      <c r="Z24" s="2"/>
+    </row>
+    <row r="25" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1104,9 +1138,9 @@
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="2"/>
+      <c r="Z25" s="2"/>
+    </row>
+    <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1131,9 +1165,9 @@
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="2"/>
+      <c r="Z26" s="2"/>
+    </row>
+    <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1158,9 +1192,9 @@
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="2"/>
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1185,9 +1219,9 @@
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2"/>
+      <c r="Z28" s="2"/>
+    </row>
+    <row r="29" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1212,9 +1246,9 @@
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="2"/>
+      <c r="Z29" s="2"/>
+    </row>
+    <row r="30" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1239,9 +1273,9 @@
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="2"/>
+      <c r="Z30" s="2"/>
+    </row>
+    <row r="31" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1266,9 +1300,9 @@
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2"/>
+      <c r="Z31" s="2"/>
+    </row>
+    <row r="32" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1293,9 +1327,9 @@
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2"/>
+      <c r="Z32" s="2"/>
+    </row>
+    <row r="33" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1320,9 +1354,9 @@
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="2"/>
+      <c r="Z33" s="2"/>
+    </row>
+    <row r="34" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1347,9 +1381,9 @@
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2"/>
+      <c r="Z34" s="2"/>
+    </row>
+    <row r="35" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1374,9 +1408,9 @@
       <c r="W35" s="2"/>
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="2"/>
+      <c r="Z35" s="2"/>
+    </row>
+    <row r="36" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1401,9 +1435,9 @@
       <c r="W36" s="2"/>
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2"/>
+      <c r="Z36" s="2"/>
+    </row>
+    <row r="37" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1428,9 +1462,9 @@
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="2"/>
+      <c r="Z37" s="2"/>
+    </row>
+    <row r="38" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1455,9 +1489,9 @@
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="2"/>
+      <c r="Z38" s="2"/>
+    </row>
+    <row r="39" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1482,9 +1516,9 @@
       <c r="W39" s="2"/>
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="2"/>
+      <c r="Z39" s="2"/>
+    </row>
+    <row r="40" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1509,9 +1543,9 @@
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="2"/>
+      <c r="Z40" s="2"/>
+    </row>
+    <row r="41" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1536,9 +1570,9 @@
       <c r="W41" s="2"/>
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="2"/>
+      <c r="Z41" s="2"/>
+    </row>
+    <row r="42" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1563,9 +1597,9 @@
       <c r="W42" s="2"/>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2"/>
+      <c r="Z42" s="2"/>
+    </row>
+    <row r="43" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1590,9 +1624,9 @@
       <c r="W43" s="2"/>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="2"/>
+      <c r="Z43" s="2"/>
+    </row>
+    <row r="44" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1617,9 +1651,9 @@
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2"/>
+      <c r="Z44" s="2"/>
+    </row>
+    <row r="45" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1644,9 +1678,9 @@
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="2"/>
+      <c r="Z45" s="2"/>
+    </row>
+    <row r="46" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1671,9 +1705,9 @@
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="2"/>
+      <c r="Z46" s="2"/>
+    </row>
+    <row r="47" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1698,9 +1732,9 @@
       <c r="W47" s="2"/>
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="2"/>
+      <c r="Z47" s="2"/>
+    </row>
+    <row r="48" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1725,9 +1759,9 @@
       <c r="W48" s="2"/>
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="2"/>
+      <c r="Z48" s="2"/>
+    </row>
+    <row r="49" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1752,9 +1786,9 @@
       <c r="W49" s="2"/>
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="2"/>
+      <c r="Z49" s="2"/>
+    </row>
+    <row r="50" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1779,9 +1813,9 @@
       <c r="W50" s="2"/>
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="2"/>
+      <c r="Z50" s="2"/>
+    </row>
+    <row r="51" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1806,9 +1840,9 @@
       <c r="W51" s="2"/>
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="2"/>
+      <c r="Z51" s="2"/>
+    </row>
+    <row r="52" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1833,9 +1867,9 @@
       <c r="W52" s="2"/>
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="2"/>
+      <c r="Z52" s="2"/>
+    </row>
+    <row r="53" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1860,9 +1894,9 @@
       <c r="W53" s="2"/>
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="2"/>
+      <c r="Z53" s="2"/>
+    </row>
+    <row r="54" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -1887,9 +1921,9 @@
       <c r="W54" s="2"/>
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="2"/>
+      <c r="Z54" s="2"/>
+    </row>
+    <row r="55" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -1914,9 +1948,9 @@
       <c r="W55" s="2"/>
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="2"/>
+      <c r="Z55" s="2"/>
+    </row>
+    <row r="56" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1941,9 +1975,9 @@
       <c r="W56" s="2"/>
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="2"/>
+      <c r="Z56" s="2"/>
+    </row>
+    <row r="57" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -1968,9 +2002,9 @@
       <c r="W57" s="2"/>
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="2"/>
+      <c r="Z57" s="2"/>
+    </row>
+    <row r="58" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -1995,9 +2029,9 @@
       <c r="W58" s="2"/>
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="2"/>
+      <c r="Z58" s="2"/>
+    </row>
+    <row r="59" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2022,9 +2056,9 @@
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="2"/>
+      <c r="Z59" s="2"/>
+    </row>
+    <row r="60" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2049,9 +2083,9 @@
       <c r="W60" s="2"/>
       <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="2"/>
+      <c r="Z60" s="2"/>
+    </row>
+    <row r="61" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2076,9 +2110,9 @@
       <c r="W61" s="2"/>
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="2"/>
+      <c r="Z61" s="2"/>
+    </row>
+    <row r="62" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2103,9 +2137,9 @@
       <c r="W62" s="2"/>
       <c r="X62" s="2"/>
       <c r="Y62" s="2"/>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="2"/>
+      <c r="Z62" s="2"/>
+    </row>
+    <row r="63" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2130,9 +2164,9 @@
       <c r="W63" s="2"/>
       <c r="X63" s="2"/>
       <c r="Y63" s="2"/>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="2"/>
+      <c r="Z63" s="2"/>
+    </row>
+    <row r="64" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2157,9 +2191,9 @@
       <c r="W64" s="2"/>
       <c r="X64" s="2"/>
       <c r="Y64" s="2"/>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="2"/>
+      <c r="Z64" s="2"/>
+    </row>
+    <row r="65" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -2184,9 +2218,9 @@
       <c r="W65" s="2"/>
       <c r="X65" s="2"/>
       <c r="Y65" s="2"/>
-    </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="2"/>
+      <c r="Z65" s="2"/>
+    </row>
+    <row r="66" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -2211,9 +2245,9 @@
       <c r="W66" s="2"/>
       <c r="X66" s="2"/>
       <c r="Y66" s="2"/>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="2"/>
+      <c r="Z66" s="2"/>
+    </row>
+    <row r="67" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -2238,9 +2272,9 @@
       <c r="W67" s="2"/>
       <c r="X67" s="2"/>
       <c r="Y67" s="2"/>
-    </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="2"/>
+      <c r="Z67" s="2"/>
+    </row>
+    <row r="68" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2265,9 +2299,9 @@
       <c r="W68" s="2"/>
       <c r="X68" s="2"/>
       <c r="Y68" s="2"/>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="2"/>
+      <c r="Z68" s="2"/>
+    </row>
+    <row r="69" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -2292,9 +2326,9 @@
       <c r="W69" s="2"/>
       <c r="X69" s="2"/>
       <c r="Y69" s="2"/>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="2"/>
+      <c r="Z69" s="2"/>
+    </row>
+    <row r="70" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2319,9 +2353,9 @@
       <c r="W70" s="2"/>
       <c r="X70" s="2"/>
       <c r="Y70" s="2"/>
-    </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="2"/>
+      <c r="Z70" s="2"/>
+    </row>
+    <row r="71" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -2346,9 +2380,9 @@
       <c r="W71" s="2"/>
       <c r="X71" s="2"/>
       <c r="Y71" s="2"/>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="2"/>
+      <c r="Z71" s="2"/>
+    </row>
+    <row r="72" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -2373,9 +2407,9 @@
       <c r="W72" s="2"/>
       <c r="X72" s="2"/>
       <c r="Y72" s="2"/>
-    </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="2"/>
+      <c r="Z72" s="2"/>
+    </row>
+    <row r="73" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -2400,9 +2434,9 @@
       <c r="W73" s="2"/>
       <c r="X73" s="2"/>
       <c r="Y73" s="2"/>
-    </row>
-    <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="2"/>
+      <c r="Z73" s="2"/>
+    </row>
+    <row r="74" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -2427,9 +2461,9 @@
       <c r="W74" s="2"/>
       <c r="X74" s="2"/>
       <c r="Y74" s="2"/>
-    </row>
-    <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="2"/>
+      <c r="Z74" s="2"/>
+    </row>
+    <row r="75" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -2454,9 +2488,9 @@
       <c r="W75" s="2"/>
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
-    </row>
-    <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="2"/>
+      <c r="Z75" s="2"/>
+    </row>
+    <row r="76" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -2481,9 +2515,9 @@
       <c r="W76" s="2"/>
       <c r="X76" s="2"/>
       <c r="Y76" s="2"/>
-    </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="2"/>
+      <c r="Z76" s="2"/>
+    </row>
+    <row r="77" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -2508,9 +2542,9 @@
       <c r="W77" s="2"/>
       <c r="X77" s="2"/>
       <c r="Y77" s="2"/>
-    </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="2"/>
+      <c r="Z77" s="2"/>
+    </row>
+    <row r="78" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -2535,9 +2569,9 @@
       <c r="W78" s="2"/>
       <c r="X78" s="2"/>
       <c r="Y78" s="2"/>
-    </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="2"/>
+      <c r="Z78" s="2"/>
+    </row>
+    <row r="79" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -2562,9 +2596,9 @@
       <c r="W79" s="2"/>
       <c r="X79" s="2"/>
       <c r="Y79" s="2"/>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="2"/>
+      <c r="Z79" s="2"/>
+    </row>
+    <row r="80" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -2589,9 +2623,9 @@
       <c r="W80" s="2"/>
       <c r="X80" s="2"/>
       <c r="Y80" s="2"/>
-    </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="2"/>
+      <c r="Z80" s="2"/>
+    </row>
+    <row r="81" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -2616,9 +2650,9 @@
       <c r="W81" s="2"/>
       <c r="X81" s="2"/>
       <c r="Y81" s="2"/>
-    </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="2"/>
+      <c r="Z81" s="2"/>
+    </row>
+    <row r="82" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -2643,9 +2677,9 @@
       <c r="W82" s="2"/>
       <c r="X82" s="2"/>
       <c r="Y82" s="2"/>
-    </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="2"/>
+      <c r="Z82" s="2"/>
+    </row>
+    <row r="83" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -2670,9 +2704,9 @@
       <c r="W83" s="2"/>
       <c r="X83" s="2"/>
       <c r="Y83" s="2"/>
-    </row>
-    <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="2"/>
+      <c r="Z83" s="2"/>
+    </row>
+    <row r="84" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -2697,9 +2731,9 @@
       <c r="W84" s="2"/>
       <c r="X84" s="2"/>
       <c r="Y84" s="2"/>
-    </row>
-    <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="2"/>
+      <c r="Z84" s="2"/>
+    </row>
+    <row r="85" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -2724,9 +2758,9 @@
       <c r="W85" s="2"/>
       <c r="X85" s="2"/>
       <c r="Y85" s="2"/>
-    </row>
-    <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="2"/>
+      <c r="Z85" s="2"/>
+    </row>
+    <row r="86" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -2751,9 +2785,9 @@
       <c r="W86" s="2"/>
       <c r="X86" s="2"/>
       <c r="Y86" s="2"/>
-    </row>
-    <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="2"/>
+      <c r="Z86" s="2"/>
+    </row>
+    <row r="87" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -2778,9 +2812,9 @@
       <c r="W87" s="2"/>
       <c r="X87" s="2"/>
       <c r="Y87" s="2"/>
-    </row>
-    <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="2"/>
+      <c r="Z87" s="2"/>
+    </row>
+    <row r="88" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -2805,9 +2839,9 @@
       <c r="W88" s="2"/>
       <c r="X88" s="2"/>
       <c r="Y88" s="2"/>
-    </row>
-    <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="2"/>
+      <c r="Z88" s="2"/>
+    </row>
+    <row r="89" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -2832,9 +2866,9 @@
       <c r="W89" s="2"/>
       <c r="X89" s="2"/>
       <c r="Y89" s="2"/>
-    </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="2"/>
+      <c r="Z89" s="2"/>
+    </row>
+    <row r="90" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -2859,9 +2893,9 @@
       <c r="W90" s="2"/>
       <c r="X90" s="2"/>
       <c r="Y90" s="2"/>
-    </row>
-    <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="2"/>
+      <c r="Z90" s="2"/>
+    </row>
+    <row r="91" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -2886,9 +2920,9 @@
       <c r="W91" s="2"/>
       <c r="X91" s="2"/>
       <c r="Y91" s="2"/>
-    </row>
-    <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="2"/>
+      <c r="Z91" s="2"/>
+    </row>
+    <row r="92" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -2913,9 +2947,9 @@
       <c r="W92" s="2"/>
       <c r="X92" s="2"/>
       <c r="Y92" s="2"/>
-    </row>
-    <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="2"/>
+      <c r="Z92" s="2"/>
+    </row>
+    <row r="93" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -2940,9 +2974,9 @@
       <c r="W93" s="2"/>
       <c r="X93" s="2"/>
       <c r="Y93" s="2"/>
-    </row>
-    <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="2"/>
+      <c r="Z93" s="2"/>
+    </row>
+    <row r="94" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -2967,9 +3001,9 @@
       <c r="W94" s="2"/>
       <c r="X94" s="2"/>
       <c r="Y94" s="2"/>
-    </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="2"/>
+      <c r="Z94" s="2"/>
+    </row>
+    <row r="95" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -2994,9 +3028,9 @@
       <c r="W95" s="2"/>
       <c r="X95" s="2"/>
       <c r="Y95" s="2"/>
-    </row>
-    <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="2"/>
+      <c r="Z95" s="2"/>
+    </row>
+    <row r="96" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -3021,9 +3055,9 @@
       <c r="W96" s="2"/>
       <c r="X96" s="2"/>
       <c r="Y96" s="2"/>
-    </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="2"/>
+      <c r="Z96" s="2"/>
+    </row>
+    <row r="97" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -3048,9 +3082,9 @@
       <c r="W97" s="2"/>
       <c r="X97" s="2"/>
       <c r="Y97" s="2"/>
-    </row>
-    <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="2"/>
+      <c r="Z97" s="2"/>
+    </row>
+    <row r="98" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -3075,9 +3109,9 @@
       <c r="W98" s="2"/>
       <c r="X98" s="2"/>
       <c r="Y98" s="2"/>
-    </row>
-    <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="2"/>
+      <c r="Z98" s="2"/>
+    </row>
+    <row r="99" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -3102,9 +3136,9 @@
       <c r="W99" s="2"/>
       <c r="X99" s="2"/>
       <c r="Y99" s="2"/>
-    </row>
-    <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="2"/>
+      <c r="Z99" s="2"/>
+    </row>
+    <row r="100" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3129,9 +3163,9 @@
       <c r="W100" s="2"/>
       <c r="X100" s="2"/>
       <c r="Y100" s="2"/>
-    </row>
-    <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="2"/>
+      <c r="Z100" s="2"/>
+    </row>
+    <row r="101" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -3156,9 +3190,9 @@
       <c r="W101" s="2"/>
       <c r="X101" s="2"/>
       <c r="Y101" s="2"/>
-    </row>
-    <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="2"/>
+      <c r="Z101" s="2"/>
+    </row>
+    <row r="102" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -3183,9 +3217,9 @@
       <c r="W102" s="2"/>
       <c r="X102" s="2"/>
       <c r="Y102" s="2"/>
-    </row>
-    <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="2"/>
+      <c r="Z102" s="2"/>
+    </row>
+    <row r="103" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -3210,9 +3244,9 @@
       <c r="W103" s="2"/>
       <c r="X103" s="2"/>
       <c r="Y103" s="2"/>
-    </row>
-    <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="2"/>
+      <c r="Z103" s="2"/>
+    </row>
+    <row r="104" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -3237,9 +3271,9 @@
       <c r="W104" s="2"/>
       <c r="X104" s="2"/>
       <c r="Y104" s="2"/>
-    </row>
-    <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="2"/>
+      <c r="Z104" s="2"/>
+    </row>
+    <row r="105" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -3264,9 +3298,9 @@
       <c r="W105" s="2"/>
       <c r="X105" s="2"/>
       <c r="Y105" s="2"/>
-    </row>
-    <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="2"/>
+      <c r="Z105" s="2"/>
+    </row>
+    <row r="106" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -3291,9 +3325,9 @@
       <c r="W106" s="2"/>
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
-    </row>
-    <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="2"/>
+      <c r="Z106" s="2"/>
+    </row>
+    <row r="107" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -3318,9 +3352,9 @@
       <c r="W107" s="2"/>
       <c r="X107" s="2"/>
       <c r="Y107" s="2"/>
-    </row>
-    <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="2"/>
+      <c r="Z107" s="2"/>
+    </row>
+    <row r="108" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -3345,9 +3379,9 @@
       <c r="W108" s="2"/>
       <c r="X108" s="2"/>
       <c r="Y108" s="2"/>
-    </row>
-    <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="2"/>
+      <c r="Z108" s="2"/>
+    </row>
+    <row r="109" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -3372,9 +3406,9 @@
       <c r="W109" s="2"/>
       <c r="X109" s="2"/>
       <c r="Y109" s="2"/>
-    </row>
-    <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="2"/>
+      <c r="Z109" s="2"/>
+    </row>
+    <row r="110" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -3399,9 +3433,9 @@
       <c r="W110" s="2"/>
       <c r="X110" s="2"/>
       <c r="Y110" s="2"/>
-    </row>
-    <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="2"/>
+      <c r="Z110" s="2"/>
+    </row>
+    <row r="111" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -3426,9 +3460,9 @@
       <c r="W111" s="2"/>
       <c r="X111" s="2"/>
       <c r="Y111" s="2"/>
-    </row>
-    <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="2"/>
+      <c r="Z111" s="2"/>
+    </row>
+    <row r="112" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -3453,9 +3487,9 @@
       <c r="W112" s="2"/>
       <c r="X112" s="2"/>
       <c r="Y112" s="2"/>
-    </row>
-    <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="2"/>
+      <c r="Z112" s="2"/>
+    </row>
+    <row r="113" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -3480,9 +3514,9 @@
       <c r="W113" s="2"/>
       <c r="X113" s="2"/>
       <c r="Y113" s="2"/>
-    </row>
-    <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="2"/>
+      <c r="Z113" s="2"/>
+    </row>
+    <row r="114" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -3507,9 +3541,9 @@
       <c r="W114" s="2"/>
       <c r="X114" s="2"/>
       <c r="Y114" s="2"/>
-    </row>
-    <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="2"/>
+      <c r="Z114" s="2"/>
+    </row>
+    <row r="115" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -3534,9 +3568,9 @@
       <c r="W115" s="2"/>
       <c r="X115" s="2"/>
       <c r="Y115" s="2"/>
-    </row>
-    <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="2"/>
+      <c r="Z115" s="2"/>
+    </row>
+    <row r="116" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -3561,9 +3595,9 @@
       <c r="W116" s="2"/>
       <c r="X116" s="2"/>
       <c r="Y116" s="2"/>
-    </row>
-    <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="2"/>
+      <c r="Z116" s="2"/>
+    </row>
+    <row r="117" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -3588,9 +3622,9 @@
       <c r="W117" s="2"/>
       <c r="X117" s="2"/>
       <c r="Y117" s="2"/>
-    </row>
-    <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="2"/>
+      <c r="Z117" s="2"/>
+    </row>
+    <row r="118" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -3615,9 +3649,9 @@
       <c r="W118" s="2"/>
       <c r="X118" s="2"/>
       <c r="Y118" s="2"/>
-    </row>
-    <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="2"/>
+      <c r="Z118" s="2"/>
+    </row>
+    <row r="119" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -3642,9 +3676,9 @@
       <c r="W119" s="2"/>
       <c r="X119" s="2"/>
       <c r="Y119" s="2"/>
-    </row>
-    <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="2"/>
+      <c r="Z119" s="2"/>
+    </row>
+    <row r="120" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -3669,9 +3703,9 @@
       <c r="W120" s="2"/>
       <c r="X120" s="2"/>
       <c r="Y120" s="2"/>
-    </row>
-    <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="2"/>
+      <c r="Z120" s="2"/>
+    </row>
+    <row r="121" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -3696,9 +3730,9 @@
       <c r="W121" s="2"/>
       <c r="X121" s="2"/>
       <c r="Y121" s="2"/>
-    </row>
-    <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="2"/>
+      <c r="Z121" s="2"/>
+    </row>
+    <row r="122" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -3723,9 +3757,9 @@
       <c r="W122" s="2"/>
       <c r="X122" s="2"/>
       <c r="Y122" s="2"/>
-    </row>
-    <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="2"/>
+      <c r="Z122" s="2"/>
+    </row>
+    <row r="123" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -3750,9 +3784,9 @@
       <c r="W123" s="2"/>
       <c r="X123" s="2"/>
       <c r="Y123" s="2"/>
-    </row>
-    <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="2"/>
+      <c r="Z123" s="2"/>
+    </row>
+    <row r="124" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -3777,9 +3811,9 @@
       <c r="W124" s="2"/>
       <c r="X124" s="2"/>
       <c r="Y124" s="2"/>
-    </row>
-    <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="2"/>
+      <c r="Z124" s="2"/>
+    </row>
+    <row r="125" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -3804,9 +3838,9 @@
       <c r="W125" s="2"/>
       <c r="X125" s="2"/>
       <c r="Y125" s="2"/>
-    </row>
-    <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="2"/>
+      <c r="Z125" s="2"/>
+    </row>
+    <row r="126" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -3831,9 +3865,9 @@
       <c r="W126" s="2"/>
       <c r="X126" s="2"/>
       <c r="Y126" s="2"/>
-    </row>
-    <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="2"/>
+      <c r="Z126" s="2"/>
+    </row>
+    <row r="127" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -3858,9 +3892,9 @@
       <c r="W127" s="2"/>
       <c r="X127" s="2"/>
       <c r="Y127" s="2"/>
-    </row>
-    <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="2"/>
+      <c r="Z127" s="2"/>
+    </row>
+    <row r="128" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -3885,9 +3919,9 @@
       <c r="W128" s="2"/>
       <c r="X128" s="2"/>
       <c r="Y128" s="2"/>
-    </row>
-    <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="2"/>
+      <c r="Z128" s="2"/>
+    </row>
+    <row r="129" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
@@ -3912,9 +3946,9 @@
       <c r="W129" s="2"/>
       <c r="X129" s="2"/>
       <c r="Y129" s="2"/>
-    </row>
-    <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="2"/>
+      <c r="Z129" s="2"/>
+    </row>
+    <row r="130" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
@@ -3939,9 +3973,9 @@
       <c r="W130" s="2"/>
       <c r="X130" s="2"/>
       <c r="Y130" s="2"/>
-    </row>
-    <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="2"/>
+      <c r="Z130" s="2"/>
+    </row>
+    <row r="131" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -3966,9 +4000,9 @@
       <c r="W131" s="2"/>
       <c r="X131" s="2"/>
       <c r="Y131" s="2"/>
-    </row>
-    <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="2"/>
+      <c r="Z131" s="2"/>
+    </row>
+    <row r="132" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -3993,9 +4027,9 @@
       <c r="W132" s="2"/>
       <c r="X132" s="2"/>
       <c r="Y132" s="2"/>
-    </row>
-    <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="2"/>
+      <c r="Z132" s="2"/>
+    </row>
+    <row r="133" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
@@ -4020,9 +4054,9 @@
       <c r="W133" s="2"/>
       <c r="X133" s="2"/>
       <c r="Y133" s="2"/>
-    </row>
-    <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="2"/>
+      <c r="Z133" s="2"/>
+    </row>
+    <row r="134" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -4047,9 +4081,9 @@
       <c r="W134" s="2"/>
       <c r="X134" s="2"/>
       <c r="Y134" s="2"/>
-    </row>
-    <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="2"/>
+      <c r="Z134" s="2"/>
+    </row>
+    <row r="135" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
@@ -4074,9 +4108,9 @@
       <c r="W135" s="2"/>
       <c r="X135" s="2"/>
       <c r="Y135" s="2"/>
-    </row>
-    <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="2"/>
+      <c r="Z135" s="2"/>
+    </row>
+    <row r="136" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -4101,9 +4135,9 @@
       <c r="W136" s="2"/>
       <c r="X136" s="2"/>
       <c r="Y136" s="2"/>
-    </row>
-    <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="2"/>
+      <c r="Z136" s="2"/>
+    </row>
+    <row r="137" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
@@ -4128,9 +4162,9 @@
       <c r="W137" s="2"/>
       <c r="X137" s="2"/>
       <c r="Y137" s="2"/>
-    </row>
-    <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="2"/>
+      <c r="Z137" s="2"/>
+    </row>
+    <row r="138" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
@@ -4155,9 +4189,9 @@
       <c r="W138" s="2"/>
       <c r="X138" s="2"/>
       <c r="Y138" s="2"/>
-    </row>
-    <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="2"/>
+      <c r="Z138" s="2"/>
+    </row>
+    <row r="139" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -4182,9 +4216,9 @@
       <c r="W139" s="2"/>
       <c r="X139" s="2"/>
       <c r="Y139" s="2"/>
-    </row>
-    <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="2"/>
+      <c r="Z139" s="2"/>
+    </row>
+    <row r="140" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -4209,9 +4243,9 @@
       <c r="W140" s="2"/>
       <c r="X140" s="2"/>
       <c r="Y140" s="2"/>
-    </row>
-    <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="2"/>
+      <c r="Z140" s="2"/>
+    </row>
+    <row r="141" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
@@ -4236,9 +4270,9 @@
       <c r="W141" s="2"/>
       <c r="X141" s="2"/>
       <c r="Y141" s="2"/>
-    </row>
-    <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="2"/>
+      <c r="Z141" s="2"/>
+    </row>
+    <row r="142" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
@@ -4263,9 +4297,9 @@
       <c r="W142" s="2"/>
       <c r="X142" s="2"/>
       <c r="Y142" s="2"/>
-    </row>
-    <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="2"/>
+      <c r="Z142" s="2"/>
+    </row>
+    <row r="143" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
@@ -4290,9 +4324,9 @@
       <c r="W143" s="2"/>
       <c r="X143" s="2"/>
       <c r="Y143" s="2"/>
-    </row>
-    <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="2"/>
+      <c r="Z143" s="2"/>
+    </row>
+    <row r="144" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
@@ -4317,9 +4351,9 @@
       <c r="W144" s="2"/>
       <c r="X144" s="2"/>
       <c r="Y144" s="2"/>
-    </row>
-    <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="2"/>
+      <c r="Z144" s="2"/>
+    </row>
+    <row r="145" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
@@ -4344,9 +4378,9 @@
       <c r="W145" s="2"/>
       <c r="X145" s="2"/>
       <c r="Y145" s="2"/>
-    </row>
-    <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="2"/>
+      <c r="Z145" s="2"/>
+    </row>
+    <row r="146" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
@@ -4371,9 +4405,9 @@
       <c r="W146" s="2"/>
       <c r="X146" s="2"/>
       <c r="Y146" s="2"/>
-    </row>
-    <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="2"/>
+      <c r="Z146" s="2"/>
+    </row>
+    <row r="147" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
@@ -4398,9 +4432,9 @@
       <c r="W147" s="2"/>
       <c r="X147" s="2"/>
       <c r="Y147" s="2"/>
-    </row>
-    <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="2"/>
+      <c r="Z147" s="2"/>
+    </row>
+    <row r="148" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
@@ -4425,9 +4459,9 @@
       <c r="W148" s="2"/>
       <c r="X148" s="2"/>
       <c r="Y148" s="2"/>
-    </row>
-    <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="2"/>
+      <c r="Z148" s="2"/>
+    </row>
+    <row r="149" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
@@ -4452,9 +4486,9 @@
       <c r="W149" s="2"/>
       <c r="X149" s="2"/>
       <c r="Y149" s="2"/>
-    </row>
-    <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="2"/>
+      <c r="Z149" s="2"/>
+    </row>
+    <row r="150" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
@@ -4479,9 +4513,9 @@
       <c r="W150" s="2"/>
       <c r="X150" s="2"/>
       <c r="Y150" s="2"/>
-    </row>
-    <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="2"/>
+      <c r="Z150" s="2"/>
+    </row>
+    <row r="151" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
@@ -4506,9 +4540,9 @@
       <c r="W151" s="2"/>
       <c r="X151" s="2"/>
       <c r="Y151" s="2"/>
-    </row>
-    <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="2"/>
+      <c r="Z151" s="2"/>
+    </row>
+    <row r="152" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
@@ -4533,9 +4567,9 @@
       <c r="W152" s="2"/>
       <c r="X152" s="2"/>
       <c r="Y152" s="2"/>
-    </row>
-    <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="2"/>
+      <c r="Z152" s="2"/>
+    </row>
+    <row r="153" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
@@ -4560,9 +4594,9 @@
       <c r="W153" s="2"/>
       <c r="X153" s="2"/>
       <c r="Y153" s="2"/>
-    </row>
-    <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="2"/>
+      <c r="Z153" s="2"/>
+    </row>
+    <row r="154" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
@@ -4587,9 +4621,9 @@
       <c r="W154" s="2"/>
       <c r="X154" s="2"/>
       <c r="Y154" s="2"/>
-    </row>
-    <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="2"/>
+      <c r="Z154" s="2"/>
+    </row>
+    <row r="155" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
@@ -4614,9 +4648,9 @@
       <c r="W155" s="2"/>
       <c r="X155" s="2"/>
       <c r="Y155" s="2"/>
-    </row>
-    <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="2"/>
+      <c r="Z155" s="2"/>
+    </row>
+    <row r="156" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -4641,9 +4675,9 @@
       <c r="W156" s="2"/>
       <c r="X156" s="2"/>
       <c r="Y156" s="2"/>
-    </row>
-    <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="2"/>
+      <c r="Z156" s="2"/>
+    </row>
+    <row r="157" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
@@ -4668,9 +4702,9 @@
       <c r="W157" s="2"/>
       <c r="X157" s="2"/>
       <c r="Y157" s="2"/>
-    </row>
-    <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="2"/>
+      <c r="Z157" s="2"/>
+    </row>
+    <row r="158" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -4695,9 +4729,9 @@
       <c r="W158" s="2"/>
       <c r="X158" s="2"/>
       <c r="Y158" s="2"/>
-    </row>
-    <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="2"/>
+      <c r="Z158" s="2"/>
+    </row>
+    <row r="159" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
@@ -4722,9 +4756,9 @@
       <c r="W159" s="2"/>
       <c r="X159" s="2"/>
       <c r="Y159" s="2"/>
-    </row>
-    <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="2"/>
+      <c r="Z159" s="2"/>
+    </row>
+    <row r="160" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
@@ -4749,9 +4783,9 @@
       <c r="W160" s="2"/>
       <c r="X160" s="2"/>
       <c r="Y160" s="2"/>
-    </row>
-    <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="2"/>
+      <c r="Z160" s="2"/>
+    </row>
+    <row r="161" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
@@ -4776,9 +4810,9 @@
       <c r="W161" s="2"/>
       <c r="X161" s="2"/>
       <c r="Y161" s="2"/>
-    </row>
-    <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="2"/>
+      <c r="Z161" s="2"/>
+    </row>
+    <row r="162" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
@@ -4803,9 +4837,9 @@
       <c r="W162" s="2"/>
       <c r="X162" s="2"/>
       <c r="Y162" s="2"/>
-    </row>
-    <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="2"/>
+      <c r="Z162" s="2"/>
+    </row>
+    <row r="163" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -4830,9 +4864,9 @@
       <c r="W163" s="2"/>
       <c r="X163" s="2"/>
       <c r="Y163" s="2"/>
-    </row>
-    <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="2"/>
+      <c r="Z163" s="2"/>
+    </row>
+    <row r="164" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
@@ -4857,9 +4891,9 @@
       <c r="W164" s="2"/>
       <c r="X164" s="2"/>
       <c r="Y164" s="2"/>
-    </row>
-    <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="2"/>
+      <c r="Z164" s="2"/>
+    </row>
+    <row r="165" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -4884,9 +4918,9 @@
       <c r="W165" s="2"/>
       <c r="X165" s="2"/>
       <c r="Y165" s="2"/>
-    </row>
-    <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="2"/>
+      <c r="Z165" s="2"/>
+    </row>
+    <row r="166" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
@@ -4911,9 +4945,9 @@
       <c r="W166" s="2"/>
       <c r="X166" s="2"/>
       <c r="Y166" s="2"/>
-    </row>
-    <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="2"/>
+      <c r="Z166" s="2"/>
+    </row>
+    <row r="167" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
@@ -4938,9 +4972,9 @@
       <c r="W167" s="2"/>
       <c r="X167" s="2"/>
       <c r="Y167" s="2"/>
-    </row>
-    <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="2"/>
+      <c r="Z167" s="2"/>
+    </row>
+    <row r="168" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
@@ -4965,9 +4999,9 @@
       <c r="W168" s="2"/>
       <c r="X168" s="2"/>
       <c r="Y168" s="2"/>
-    </row>
-    <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="2"/>
+      <c r="Z168" s="2"/>
+    </row>
+    <row r="169" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -4992,9 +5026,9 @@
       <c r="W169" s="2"/>
       <c r="X169" s="2"/>
       <c r="Y169" s="2"/>
-    </row>
-    <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="2"/>
+      <c r="Z169" s="2"/>
+    </row>
+    <row r="170" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -5019,9 +5053,9 @@
       <c r="W170" s="2"/>
       <c r="X170" s="2"/>
       <c r="Y170" s="2"/>
-    </row>
-    <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="2"/>
+      <c r="Z170" s="2"/>
+    </row>
+    <row r="171" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -5046,9 +5080,9 @@
       <c r="W171" s="2"/>
       <c r="X171" s="2"/>
       <c r="Y171" s="2"/>
-    </row>
-    <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="2"/>
+      <c r="Z171" s="2"/>
+    </row>
+    <row r="172" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -5073,9 +5107,9 @@
       <c r="W172" s="2"/>
       <c r="X172" s="2"/>
       <c r="Y172" s="2"/>
-    </row>
-    <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="2"/>
+      <c r="Z172" s="2"/>
+    </row>
+    <row r="173" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -5100,9 +5134,9 @@
       <c r="W173" s="2"/>
       <c r="X173" s="2"/>
       <c r="Y173" s="2"/>
-    </row>
-    <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="2"/>
+      <c r="Z173" s="2"/>
+    </row>
+    <row r="174" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
@@ -5127,9 +5161,9 @@
       <c r="W174" s="2"/>
       <c r="X174" s="2"/>
       <c r="Y174" s="2"/>
-    </row>
-    <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="2"/>
+      <c r="Z174" s="2"/>
+    </row>
+    <row r="175" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -5154,9 +5188,9 @@
       <c r="W175" s="2"/>
       <c r="X175" s="2"/>
       <c r="Y175" s="2"/>
-    </row>
-    <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="2"/>
+      <c r="Z175" s="2"/>
+    </row>
+    <row r="176" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
@@ -5181,9 +5215,9 @@
       <c r="W176" s="2"/>
       <c r="X176" s="2"/>
       <c r="Y176" s="2"/>
-    </row>
-    <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="2"/>
+      <c r="Z176" s="2"/>
+    </row>
+    <row r="177" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
@@ -5208,9 +5242,9 @@
       <c r="W177" s="2"/>
       <c r="X177" s="2"/>
       <c r="Y177" s="2"/>
-    </row>
-    <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="2"/>
+      <c r="Z177" s="2"/>
+    </row>
+    <row r="178" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
@@ -5235,9 +5269,9 @@
       <c r="W178" s="2"/>
       <c r="X178" s="2"/>
       <c r="Y178" s="2"/>
-    </row>
-    <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="2"/>
+      <c r="Z178" s="2"/>
+    </row>
+    <row r="179" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
@@ -5262,9 +5296,9 @@
       <c r="W179" s="2"/>
       <c r="X179" s="2"/>
       <c r="Y179" s="2"/>
-    </row>
-    <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="2"/>
+      <c r="Z179" s="2"/>
+    </row>
+    <row r="180" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
@@ -5289,9 +5323,9 @@
       <c r="W180" s="2"/>
       <c r="X180" s="2"/>
       <c r="Y180" s="2"/>
-    </row>
-    <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="2"/>
+      <c r="Z180" s="2"/>
+    </row>
+    <row r="181" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
@@ -5316,9 +5350,9 @@
       <c r="W181" s="2"/>
       <c r="X181" s="2"/>
       <c r="Y181" s="2"/>
-    </row>
-    <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="2"/>
+      <c r="Z181" s="2"/>
+    </row>
+    <row r="182" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
@@ -5343,9 +5377,9 @@
       <c r="W182" s="2"/>
       <c r="X182" s="2"/>
       <c r="Y182" s="2"/>
-    </row>
-    <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="2"/>
+      <c r="Z182" s="2"/>
+    </row>
+    <row r="183" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
@@ -5370,9 +5404,9 @@
       <c r="W183" s="2"/>
       <c r="X183" s="2"/>
       <c r="Y183" s="2"/>
-    </row>
-    <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="2"/>
+      <c r="Z183" s="2"/>
+    </row>
+    <row r="184" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
@@ -5397,9 +5431,9 @@
       <c r="W184" s="2"/>
       <c r="X184" s="2"/>
       <c r="Y184" s="2"/>
-    </row>
-    <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="2"/>
+      <c r="Z184" s="2"/>
+    </row>
+    <row r="185" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
@@ -5424,9 +5458,9 @@
       <c r="W185" s="2"/>
       <c r="X185" s="2"/>
       <c r="Y185" s="2"/>
-    </row>
-    <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="2"/>
+      <c r="Z185" s="2"/>
+    </row>
+    <row r="186" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
@@ -5451,9 +5485,9 @@
       <c r="W186" s="2"/>
       <c r="X186" s="2"/>
       <c r="Y186" s="2"/>
-    </row>
-    <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="2"/>
+      <c r="Z186" s="2"/>
+    </row>
+    <row r="187" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
@@ -5478,9 +5512,9 @@
       <c r="W187" s="2"/>
       <c r="X187" s="2"/>
       <c r="Y187" s="2"/>
-    </row>
-    <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="2"/>
+      <c r="Z187" s="2"/>
+    </row>
+    <row r="188" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
@@ -5505,9 +5539,9 @@
       <c r="W188" s="2"/>
       <c r="X188" s="2"/>
       <c r="Y188" s="2"/>
-    </row>
-    <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="2"/>
+      <c r="Z188" s="2"/>
+    </row>
+    <row r="189" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
@@ -5532,9 +5566,9 @@
       <c r="W189" s="2"/>
       <c r="X189" s="2"/>
       <c r="Y189" s="2"/>
-    </row>
-    <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="2"/>
+      <c r="Z189" s="2"/>
+    </row>
+    <row r="190" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
@@ -5559,9 +5593,9 @@
       <c r="W190" s="2"/>
       <c r="X190" s="2"/>
       <c r="Y190" s="2"/>
-    </row>
-    <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="2"/>
+      <c r="Z190" s="2"/>
+    </row>
+    <row r="191" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
@@ -5586,9 +5620,9 @@
       <c r="W191" s="2"/>
       <c r="X191" s="2"/>
       <c r="Y191" s="2"/>
-    </row>
-    <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="2"/>
+      <c r="Z191" s="2"/>
+    </row>
+    <row r="192" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
@@ -5613,9 +5647,9 @@
       <c r="W192" s="2"/>
       <c r="X192" s="2"/>
       <c r="Y192" s="2"/>
-    </row>
-    <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="2"/>
+      <c r="Z192" s="2"/>
+    </row>
+    <row r="193" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
@@ -5640,9 +5674,9 @@
       <c r="W193" s="2"/>
       <c r="X193" s="2"/>
       <c r="Y193" s="2"/>
-    </row>
-    <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="2"/>
+      <c r="Z193" s="2"/>
+    </row>
+    <row r="194" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
@@ -5667,9 +5701,9 @@
       <c r="W194" s="2"/>
       <c r="X194" s="2"/>
       <c r="Y194" s="2"/>
-    </row>
-    <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="2"/>
+      <c r="Z194" s="2"/>
+    </row>
+    <row r="195" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
@@ -5694,9 +5728,9 @@
       <c r="W195" s="2"/>
       <c r="X195" s="2"/>
       <c r="Y195" s="2"/>
-    </row>
-    <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="2"/>
+      <c r="Z195" s="2"/>
+    </row>
+    <row r="196" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
@@ -5721,9 +5755,9 @@
       <c r="W196" s="2"/>
       <c r="X196" s="2"/>
       <c r="Y196" s="2"/>
-    </row>
-    <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="2"/>
+      <c r="Z196" s="2"/>
+    </row>
+    <row r="197" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
@@ -5748,9 +5782,9 @@
       <c r="W197" s="2"/>
       <c r="X197" s="2"/>
       <c r="Y197" s="2"/>
-    </row>
-    <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="2"/>
+      <c r="Z197" s="2"/>
+    </row>
+    <row r="198" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
@@ -5775,9 +5809,9 @@
       <c r="W198" s="2"/>
       <c r="X198" s="2"/>
       <c r="Y198" s="2"/>
-    </row>
-    <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="2"/>
+      <c r="Z198" s="2"/>
+    </row>
+    <row r="199" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
@@ -5802,9 +5836,9 @@
       <c r="W199" s="2"/>
       <c r="X199" s="2"/>
       <c r="Y199" s="2"/>
-    </row>
-    <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="2"/>
+      <c r="Z199" s="2"/>
+    </row>
+    <row r="200" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
@@ -5829,9 +5863,9 @@
       <c r="W200" s="2"/>
       <c r="X200" s="2"/>
       <c r="Y200" s="2"/>
-    </row>
-    <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="2"/>
+      <c r="Z200" s="2"/>
+    </row>
+    <row r="201" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
@@ -5856,9 +5890,9 @@
       <c r="W201" s="2"/>
       <c r="X201" s="2"/>
       <c r="Y201" s="2"/>
-    </row>
-    <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="2"/>
+      <c r="Z201" s="2"/>
+    </row>
+    <row r="202" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
@@ -5883,9 +5917,9 @@
       <c r="W202" s="2"/>
       <c r="X202" s="2"/>
       <c r="Y202" s="2"/>
-    </row>
-    <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="2"/>
+      <c r="Z202" s="2"/>
+    </row>
+    <row r="203" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
@@ -5910,9 +5944,9 @@
       <c r="W203" s="2"/>
       <c r="X203" s="2"/>
       <c r="Y203" s="2"/>
-    </row>
-    <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="2"/>
+      <c r="Z203" s="2"/>
+    </row>
+    <row r="204" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
@@ -5937,9 +5971,9 @@
       <c r="W204" s="2"/>
       <c r="X204" s="2"/>
       <c r="Y204" s="2"/>
-    </row>
-    <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="2"/>
+      <c r="Z204" s="2"/>
+    </row>
+    <row r="205" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
@@ -5964,9 +5998,9 @@
       <c r="W205" s="2"/>
       <c r="X205" s="2"/>
       <c r="Y205" s="2"/>
-    </row>
-    <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="2"/>
+      <c r="Z205" s="2"/>
+    </row>
+    <row r="206" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
@@ -5991,9 +6025,9 @@
       <c r="W206" s="2"/>
       <c r="X206" s="2"/>
       <c r="Y206" s="2"/>
-    </row>
-    <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="2"/>
+      <c r="Z206" s="2"/>
+    </row>
+    <row r="207" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
@@ -6018,9 +6052,9 @@
       <c r="W207" s="2"/>
       <c r="X207" s="2"/>
       <c r="Y207" s="2"/>
-    </row>
-    <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="2"/>
+      <c r="Z207" s="2"/>
+    </row>
+    <row r="208" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
@@ -6045,9 +6079,9 @@
       <c r="W208" s="2"/>
       <c r="X208" s="2"/>
       <c r="Y208" s="2"/>
-    </row>
-    <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="2"/>
+      <c r="Z208" s="2"/>
+    </row>
+    <row r="209" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
@@ -6072,9 +6106,9 @@
       <c r="W209" s="2"/>
       <c r="X209" s="2"/>
       <c r="Y209" s="2"/>
-    </row>
-    <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="2"/>
+      <c r="Z209" s="2"/>
+    </row>
+    <row r="210" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
@@ -6099,9 +6133,9 @@
       <c r="W210" s="2"/>
       <c r="X210" s="2"/>
       <c r="Y210" s="2"/>
-    </row>
-    <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="2"/>
+      <c r="Z210" s="2"/>
+    </row>
+    <row r="211" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
@@ -6126,9 +6160,9 @@
       <c r="W211" s="2"/>
       <c r="X211" s="2"/>
       <c r="Y211" s="2"/>
-    </row>
-    <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="2"/>
+      <c r="Z211" s="2"/>
+    </row>
+    <row r="212" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
@@ -6153,9 +6187,9 @@
       <c r="W212" s="2"/>
       <c r="X212" s="2"/>
       <c r="Y212" s="2"/>
-    </row>
-    <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="2"/>
+      <c r="Z212" s="2"/>
+    </row>
+    <row r="213" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
@@ -6180,9 +6214,9 @@
       <c r="W213" s="2"/>
       <c r="X213" s="2"/>
       <c r="Y213" s="2"/>
-    </row>
-    <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="2"/>
+      <c r="Z213" s="2"/>
+    </row>
+    <row r="214" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
@@ -6207,9 +6241,9 @@
       <c r="W214" s="2"/>
       <c r="X214" s="2"/>
       <c r="Y214" s="2"/>
-    </row>
-    <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="2"/>
+      <c r="Z214" s="2"/>
+    </row>
+    <row r="215" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
@@ -6234,9 +6268,9 @@
       <c r="W215" s="2"/>
       <c r="X215" s="2"/>
       <c r="Y215" s="2"/>
-    </row>
-    <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="2"/>
+      <c r="Z215" s="2"/>
+    </row>
+    <row r="216" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
@@ -6261,9 +6295,9 @@
       <c r="W216" s="2"/>
       <c r="X216" s="2"/>
       <c r="Y216" s="2"/>
-    </row>
-    <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="2"/>
+      <c r="Z216" s="2"/>
+    </row>
+    <row r="217" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
@@ -6288,9 +6322,9 @@
       <c r="W217" s="2"/>
       <c r="X217" s="2"/>
       <c r="Y217" s="2"/>
-    </row>
-    <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="2"/>
+      <c r="Z217" s="2"/>
+    </row>
+    <row r="218" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
@@ -6315,9 +6349,9 @@
       <c r="W218" s="2"/>
       <c r="X218" s="2"/>
       <c r="Y218" s="2"/>
-    </row>
-    <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="2"/>
+      <c r="Z218" s="2"/>
+    </row>
+    <row r="219" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
@@ -6342,9 +6376,9 @@
       <c r="W219" s="2"/>
       <c r="X219" s="2"/>
       <c r="Y219" s="2"/>
-    </row>
-    <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="2"/>
+      <c r="Z219" s="2"/>
+    </row>
+    <row r="220" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
@@ -6369,793 +6403,794 @@
       <c r="W220" s="2"/>
       <c r="X220" s="2"/>
       <c r="Y220" s="2"/>
-    </row>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+      <c r="Z220" s="2"/>
+    </row>
+    <row r="221" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
-    <hyperlink r:id="rId2" ref="G3"/>
-    <hyperlink r:id="rId3" ref="G4"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update Carga-de-Horarios.xlsx template with new data
</commit_message>
<xml_diff>
--- a/public/templates/Carga-de-Horarios.xlsx
+++ b/public/templates/Carga-de-Horarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoArDiTo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoArDiTo\Dev\proyectos\sga-uni\SGAuni-Frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B140B2C-B169-4BD4-BC6A-F9B69325F6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5479090-3E5F-468C-8698-664ED4901BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Código Curso</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>ABCEXCEL2</t>
+  </si>
+  <si>
+    <t>Fecha Inicio</t>
+  </si>
+  <si>
+    <t>Fecha Fin</t>
   </si>
 </sst>
 </file>
@@ -157,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,6 +189,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -405,8 +414,8 @@
   </sheetPr>
   <dimension ref="A1:V999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -446,8 +455,12 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="J1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -488,8 +501,12 @@
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="J2" s="10">
+        <v>45719</v>
+      </c>
+      <c r="K2" s="10">
+        <v>45750</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -530,8 +547,12 @@
       <c r="I3" s="2">
         <v>2</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="10">
+        <v>45719</v>
+      </c>
+      <c r="K3" s="10">
+        <v>45750</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -570,8 +591,12 @@
         <v>9</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="10">
+        <v>45721</v>
+      </c>
+      <c r="K4" s="10">
+        <v>45752</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>

</xml_diff>